<commit_message>
update distance range to 20m, dimeter
</commit_message>
<xml_diff>
--- a/assets/LocationPreset.xlsx
+++ b/assets/LocationPreset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\My Works\Neko-App\App\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09365C00-1391-44A3-A5D9-B8BE4F5D6962}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65EFD65B-4663-46A0-AFF9-1F22AA1B3E95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{485EAEBA-1BD5-42A4-A8A8-B4F64E392D70}"/>
   </bookViews>
@@ -57,7 +57,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -83,6 +83,12 @@
       <name val="Cordia New"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Cordia New"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -104,7 +110,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -112,9 +118,24 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -453,18 +474,18 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.77734375" customWidth="1"/>
-    <col min="2" max="2" width="17.88671875" customWidth="1"/>
-    <col min="3" max="3" width="17.77734375" customWidth="1"/>
+    <col min="1" max="1" width="17.77734375" style="8" customWidth="1"/>
+    <col min="2" max="2" width="17.88671875" style="9" customWidth="1"/>
+    <col min="3" max="3" width="17.77734375" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" ht="20.399999999999999" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -475,21 +496,21 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="42" x14ac:dyDescent="0.6">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="3">
-        <v>16.834810999999998</v>
-      </c>
-      <c r="C2" s="4">
-        <v>100.213294</v>
+      <c r="B2" s="4">
+        <v>16.834817399999999</v>
+      </c>
+      <c r="C2" s="3">
+        <v>100.2132551</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="42" x14ac:dyDescent="0.6">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="5">
         <v>16.835243999999999</v>
       </c>
       <c r="C3" s="2">

</xml_diff>